<commit_message>
- Data update from DGS's 2021/08/11 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/08/09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/08/11</t>
   </si>
 </sst>
 </file>
@@ -333,13 +336,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
+      <selection pane="topLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1452,6 +1455,23 @@
         <v>0.93</v>
       </c>
     </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="2" t="n">
+        <v>326.5</v>
+      </c>
+      <c r="C66" s="2" t="n">
+        <v>331.6</v>
+      </c>
+      <c r="D66" s="2" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>0.94</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/08/13 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/08/11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/08/13</t>
   </si>
 </sst>
 </file>
@@ -336,13 +339,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1472,6 +1475,23 @@
         <v>0.94</v>
       </c>
     </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="2" t="n">
+        <v>319.9</v>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>324.6</v>
+      </c>
+      <c r="D67" s="2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>0.95</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/08/15 and 2021/08/16 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/08/13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/08/16</t>
   </si>
 </sst>
 </file>
@@ -339,13 +342,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1492,6 +1495,23 @@
         <v>0.95</v>
       </c>
     </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" s="2" t="n">
+        <v>314.5</v>
+      </c>
+      <c r="C68" s="2" t="n">
+        <v>318.8</v>
+      </c>
+      <c r="D68" s="2" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>0.96</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/08/19 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/08/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/08/18</t>
   </si>
 </sst>
 </file>
@@ -342,13 +345,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1512,6 +1515,23 @@
         <v>0.96</v>
       </c>
     </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="2" t="n">
+        <v>314.6</v>
+      </c>
+      <c r="C69" s="2" t="n">
+        <v>319</v>
+      </c>
+      <c r="D69" s="2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/08/20 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/08/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/08/20</t>
   </si>
 </sst>
 </file>
@@ -345,13 +348,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A71" activeCellId="0" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1532,6 +1535,23 @@
         <v>0.98</v>
       </c>
     </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" s="2" t="n">
+        <v>312.3</v>
+      </c>
+      <c r="C70" s="2" t="n">
+        <v>316.6</v>
+      </c>
+      <c r="D70" s="2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/08/23 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/08/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/08/23</t>
   </si>
 </sst>
 </file>
@@ -348,13 +351,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A71" activeCellId="0" sqref="A71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1552,6 +1555,23 @@
         <v>0.98</v>
       </c>
     </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="2" t="n">
+        <v>310.4</v>
+      </c>
+      <c r="C71" s="2" t="n">
+        <v>314.6</v>
+      </c>
+      <c r="D71" s="2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/08/25 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/08/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/08/25</t>
   </si>
 </sst>
 </file>
@@ -351,13 +354,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
+      <selection pane="topLeft" activeCell="A73" activeCellId="0" sqref="A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1572,6 +1575,23 @@
         <v>0.98</v>
       </c>
     </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" s="2" t="n">
+        <v>312.8</v>
+      </c>
+      <c r="C72" s="2" t="n">
+        <v>317.1</v>
+      </c>
+      <c r="D72" s="2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E72" s="2" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/08/27 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/08/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/08/27</t>
   </si>
 </sst>
 </file>
@@ -354,13 +357,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A73" activeCellId="0" sqref="A73"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1592,6 +1595,23 @@
         <v>0.98</v>
       </c>
     </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" s="2" t="n">
+        <v>312.7</v>
+      </c>
+      <c r="C73" s="2" t="n">
+        <v>317.7</v>
+      </c>
+      <c r="D73" s="2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="E73" s="2" t="n">
+        <v>0.99</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/08/30 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/08/27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/08/30</t>
   </si>
 </sst>
 </file>
@@ -357,13 +360,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1612,6 +1615,23 @@
         <v>0.99</v>
       </c>
     </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" s="2" t="n">
+        <v>297.7</v>
+      </c>
+      <c r="C74" s="2" t="n">
+        <v>303.3</v>
+      </c>
+      <c r="D74" s="2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E74" s="2" t="n">
+        <v>0.99</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/08/31 and 2021/09/01 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/08/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/01</t>
   </si>
 </sst>
 </file>
@@ -360,13 +363,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
+      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1632,6 +1635,23 @@
         <v>0.99</v>
       </c>
     </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" s="2" t="n">
+        <v>303.5</v>
+      </c>
+      <c r="C75" s="2" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E75" s="2" t="n">
+        <v>0.99</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/03 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/09/03</t>
   </si>
 </sst>
 </file>
@@ -363,13 +366,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1652,6 +1655,23 @@
         <v>0.99</v>
       </c>
     </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" s="2" t="n">
+        <v>295.5</v>
+      </c>
+      <c r="C76" s="2" t="n">
+        <v>302.6</v>
+      </c>
+      <c r="D76" s="2" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="E76" s="2" t="n">
+        <v>0.97</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/06 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -259,7 +259,10 @@
     <t xml:space="preserve">2021/09/01</t>
   </si>
   <si>
-    <t xml:space="preserve">2020/09/03</t>
+    <t xml:space="preserve">2021/09/03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/06</t>
   </si>
 </sst>
 </file>
@@ -366,13 +369,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
+      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1672,6 +1675,23 @@
         <v>0.97</v>
       </c>
     </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" s="2" t="n">
+        <v>276</v>
+      </c>
+      <c r="C77" s="2" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="E77" s="2" t="n">
+        <v>0.93</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/08 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/08</t>
   </si>
 </sst>
 </file>
@@ -369,13 +372,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
+      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1692,6 +1695,23 @@
         <v>0.93</v>
       </c>
     </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" s="2" t="n">
+        <v>259.6</v>
+      </c>
+      <c r="C78" s="2" t="n">
+        <v>267.4</v>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="E78" s="2" t="n">
+        <v>0.93</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/10 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/10</t>
   </si>
 </sst>
 </file>
@@ -372,13 +375,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1712,6 +1715,23 @@
         <v>0.93</v>
       </c>
     </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" s="2" t="n">
+        <v>240.7</v>
+      </c>
+      <c r="C79" s="2" t="n">
+        <v>247.9</v>
+      </c>
+      <c r="D79" s="2" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="E79" s="2" t="n">
+        <v>0.87</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/13 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/13</t>
   </si>
 </sst>
 </file>
@@ -375,13 +378,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
+      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1732,6 +1735,23 @@
         <v>0.87</v>
       </c>
     </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" s="2" t="n">
+        <v>208.3</v>
+      </c>
+      <c r="C80" s="2" t="n">
+        <v>214</v>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E80" s="2" t="n">
+        <v>0.84</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/14 and 2021/09/15 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/15</t>
   </si>
 </sst>
 </file>
@@ -378,13 +381,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1752,6 +1755,23 @@
         <v>0.84</v>
       </c>
     </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" s="2" t="n">
+        <v>191.1</v>
+      </c>
+      <c r="C81" s="2" t="n">
+        <v>196.1</v>
+      </c>
+      <c r="D81" s="2" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="E81" s="2" t="n">
+        <v>0.83</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/17 and 2021/09/18 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/17</t>
   </si>
 </sst>
 </file>
@@ -381,13 +384,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1772,6 +1775,23 @@
         <v>0.83</v>
       </c>
     </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" s="2" t="n">
+        <v>173.6</v>
+      </c>
+      <c r="C82" s="2" t="n">
+        <v>177.9</v>
+      </c>
+      <c r="D82" s="2" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="E82" s="2" t="n">
+        <v>0.82</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/20 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/20</t>
   </si>
 </sst>
 </file>
@@ -384,13 +387,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
+      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1792,6 +1795,23 @@
         <v>0.82</v>
       </c>
     </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" s="2" t="n">
+        <v>149.1</v>
+      </c>
+      <c r="C83" s="2" t="n">
+        <v>152.4</v>
+      </c>
+      <c r="D83" s="2" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="E83" s="2" t="n">
+        <v>0.81</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/22 and 2021/09/23 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -281,6 +281,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/22</t>
   </si>
 </sst>
 </file>
@@ -387,13 +390,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
+      <selection pane="topLeft" activeCell="A85" activeCellId="0" sqref="A85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1812,6 +1815,23 @@
         <v>0.81</v>
       </c>
     </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="2" t="n">
+        <v>137.4</v>
+      </c>
+      <c r="C84" s="2" t="n">
+        <v>140.1</v>
+      </c>
+      <c r="D84" s="2" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>0.81</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/24 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/24</t>
   </si>
 </sst>
 </file>
@@ -390,13 +393,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A85" activeCellId="0" sqref="A85"/>
+      <selection pane="topLeft" activeCell="A86" activeCellId="0" sqref="A86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1832,6 +1835,23 @@
         <v>0.81</v>
       </c>
     </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" s="2" t="n">
+        <v>127.3</v>
+      </c>
+      <c r="C85" s="2" t="n">
+        <v>129.7</v>
+      </c>
+      <c r="D85" s="2" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="E85" s="2" t="n">
+        <v>0.82</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/25, 2021/09/26 and 2021/09/27 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/27</t>
   </si>
 </sst>
 </file>
@@ -393,13 +396,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A86" activeCellId="0" sqref="A86"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1852,6 +1855,23 @@
         <v>0.82</v>
       </c>
     </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" s="2" t="n">
+        <v>111.6</v>
+      </c>
+      <c r="C86" s="2" t="n">
+        <v>113.5</v>
+      </c>
+      <c r="D86" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>0.84</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/09/29 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/09/29</t>
   </si>
 </sst>
 </file>
@@ -396,13 +399,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
+      <selection pane="topLeft" activeCell="A88" activeCellId="0" sqref="A88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1872,6 +1875,23 @@
         <v>0.84</v>
       </c>
     </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" s="2" t="n">
+        <v>105.6</v>
+      </c>
+      <c r="C87" s="2" t="n">
+        <v>107.3</v>
+      </c>
+      <c r="D87" s="2" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="E87" s="2" t="n">
+        <v>0.87</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/01 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/09/29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/01</t>
   </si>
 </sst>
 </file>
@@ -399,13 +402,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A88" activeCellId="0" sqref="A88"/>
+      <selection pane="topLeft" activeCell="A89" activeCellId="0" sqref="A89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1892,6 +1895,23 @@
         <v>0.87</v>
       </c>
     </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" s="2" t="n">
+        <v>101.7</v>
+      </c>
+      <c r="C88" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="D88" s="2" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/04 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/04</t>
   </si>
 </sst>
 </file>
@@ -402,13 +405,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A89" activeCellId="0" sqref="A89"/>
+      <selection pane="topLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1912,6 +1915,23 @@
         <v>0.89</v>
       </c>
     </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89" s="2" t="n">
+        <v>94.3</v>
+      </c>
+      <c r="C89" s="2" t="n">
+        <v>95.1</v>
+      </c>
+      <c r="D89" s="2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="E89" s="2" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/06 and 2021/10/07 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/06</t>
   </si>
 </sst>
 </file>
@@ -405,13 +408,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
+      <selection pane="topLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1932,6 +1935,23 @@
         <v>0.9</v>
       </c>
     </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" s="2" t="n">
+        <v>90.5</v>
+      </c>
+      <c r="C90" s="2" t="n">
+        <v>90.9</v>
+      </c>
+      <c r="D90" s="2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/08 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/08</t>
   </si>
 </sst>
 </file>
@@ -408,13 +411,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
+      <selection pane="topLeft" activeCell="A92" activeCellId="0" sqref="A92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1952,6 +1955,23 @@
         <v>0.9</v>
       </c>
     </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91" s="2" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="C91" s="2" t="n">
+        <v>86.7</v>
+      </c>
+      <c r="D91" s="2" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="E91" s="2" t="n">
+        <v>0.91</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/11 and 2021/10/12 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/11</t>
   </si>
 </sst>
 </file>
@@ -411,13 +414,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A92" activeCellId="0" sqref="A92"/>
+      <selection pane="topLeft" activeCell="A93" activeCellId="0" sqref="A93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1972,6 +1975,23 @@
         <v>0.91</v>
       </c>
     </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" s="2" t="n">
+        <v>82.9</v>
+      </c>
+      <c r="C92" s="2" t="n">
+        <v>82.7</v>
+      </c>
+      <c r="D92" s="2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>0.95</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/13 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/13</t>
   </si>
 </sst>
 </file>
@@ -414,13 +417,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A93" activeCellId="0" sqref="A93"/>
+      <selection pane="topLeft" activeCell="A94" activeCellId="0" sqref="A94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -1992,6 +1995,23 @@
         <v>0.95</v>
       </c>
     </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" s="2" t="n">
+        <v>83.2</v>
+      </c>
+      <c r="C93" s="2" t="n">
+        <v>83.2</v>
+      </c>
+      <c r="D93" s="2" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="E93" s="2" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/14 and 2021/10/15 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/15</t>
   </si>
 </sst>
 </file>
@@ -417,13 +420,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A94" activeCellId="0" sqref="A94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2012,6 +2015,23 @@
         <v>0.98</v>
       </c>
     </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94" s="2" t="n">
+        <v>84.2</v>
+      </c>
+      <c r="C94" s="2" t="n">
+        <v>84.4</v>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/18 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/18</t>
   </si>
 </sst>
 </file>
@@ -420,13 +423,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
+      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2032,6 +2035,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" s="2" t="n">
+        <v>84.3</v>
+      </c>
+      <c r="C95" s="2" t="n">
+        <v>84.7</v>
+      </c>
+      <c r="D95" s="2" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="E95" s="2" t="n">
+        <v>1.02</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/20, 2021/10/21 and 2021/10/22 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -317,6 +317,12 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/22</t>
   </si>
 </sst>
 </file>
@@ -423,13 +429,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
+      <selection pane="topLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2052,6 +2058,40 @@
         <v>1.02</v>
       </c>
     </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B96" s="2" t="n">
+        <v>84.4</v>
+      </c>
+      <c r="C96" s="2" t="n">
+        <v>84.8</v>
+      </c>
+      <c r="D96" s="2" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B97" s="2" t="n">
+        <v>86.1</v>
+      </c>
+      <c r="C97" s="2" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="D97" s="2" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>1.02</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/25 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/25</t>
   </si>
 </sst>
 </file>
@@ -429,13 +432,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A99" activeCellId="0" sqref="A99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2092,6 +2095,23 @@
         <v>1.02</v>
       </c>
     </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B98" s="2" t="n">
+        <v>92.4</v>
+      </c>
+      <c r="C98" s="2" t="n">
+        <v>92.8</v>
+      </c>
+      <c r="D98" s="2" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>1.06</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/27 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/27</t>
   </si>
 </sst>
 </file>
@@ -432,13 +435,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A99" activeCellId="0" sqref="A99"/>
+      <selection pane="topLeft" activeCell="A100" activeCellId="0" sqref="A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2112,6 +2115,23 @@
         <v>1.06</v>
       </c>
     </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B99" s="2" t="n">
+        <v>94.8</v>
+      </c>
+      <c r="C99" s="2" t="n">
+        <v>94.9</v>
+      </c>
+      <c r="D99" s="2" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="E99" s="2" t="n">
+        <v>1.08</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/29 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/10/29</t>
   </si>
 </sst>
 </file>
@@ -435,13 +438,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A100" activeCellId="0" sqref="A100"/>
+      <selection pane="topLeft" activeCell="A101" activeCellId="0" sqref="A101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2132,6 +2135,23 @@
         <v>1.08</v>
       </c>
     </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B100" s="2" t="n">
+        <v>97.4</v>
+      </c>
+      <c r="C100" s="2" t="n">
+        <v>97.6</v>
+      </c>
+      <c r="D100" s="2" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="E100" s="2" t="n">
+        <v>1.08</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/10/31 and 2021/11/01 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/10/29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/01</t>
   </si>
 </sst>
 </file>
@@ -438,13 +441,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A101" activeCellId="0" sqref="A101"/>
+      <selection pane="topLeft" activeCell="A102" activeCellId="0" sqref="A102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2152,6 +2155,23 @@
         <v>1.08</v>
       </c>
     </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101" s="2" t="n">
+        <v>101.5</v>
+      </c>
+      <c r="C101" s="2" t="n">
+        <v>101.9</v>
+      </c>
+      <c r="D101" s="2" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="E101" s="2" t="n">
+        <v>1.05</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/03 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/03</t>
   </si>
 </sst>
 </file>
@@ -441,13 +444,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A102" activeCellId="0" sqref="A102"/>
+      <selection pane="topLeft" activeCell="A103" activeCellId="0" sqref="A103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2172,6 +2175,23 @@
         <v>1.05</v>
       </c>
     </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B102" s="2" t="n">
+        <v>104.3</v>
+      </c>
+      <c r="C102" s="2" t="n">
+        <v>104.4</v>
+      </c>
+      <c r="D102" s="2" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="E102" s="2" t="n">
+        <v>1.03</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/04 and 2021/11/05 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/05</t>
   </si>
 </sst>
 </file>
@@ -444,13 +447,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A103" activeCellId="0" sqref="A103"/>
+      <selection pane="topLeft" activeCell="A104" activeCellId="0" sqref="A104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2192,6 +2195,23 @@
         <v>1.03</v>
       </c>
     </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B103" s="2" t="n">
+        <v>106.1</v>
+      </c>
+      <c r="C103" s="2" t="n">
+        <v>105.6</v>
+      </c>
+      <c r="D103" s="2" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="E103" s="2" t="n">
+        <v>1.03</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/08 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/08</t>
   </si>
 </sst>
 </file>
@@ -447,13 +450,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A104" activeCellId="0" sqref="A104"/>
+      <selection pane="topLeft" activeCell="A105" activeCellId="0" sqref="A105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2212,6 +2215,23 @@
         <v>1.03</v>
       </c>
     </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B104" s="2" t="n">
+        <v>116.9</v>
+      </c>
+      <c r="C104" s="2" t="n">
+        <v>116.4</v>
+      </c>
+      <c r="D104" s="2" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="E104" s="2" t="n">
+        <v>1.08</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/10 and 2021/11/11 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/10</t>
   </si>
 </sst>
 </file>
@@ -450,13 +453,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A105" activeCellId="0" sqref="A105"/>
+      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2232,6 +2235,23 @@
         <v>1.08</v>
       </c>
     </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B105" s="2" t="n">
+        <v>125.4</v>
+      </c>
+      <c r="C105" s="2" t="n">
+        <v>124.8</v>
+      </c>
+      <c r="D105" s="2" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="E105" s="2" t="n">
+        <v>1.12</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/12 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/12</t>
   </si>
 </sst>
 </file>
@@ -453,13 +456,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
+      <selection pane="topLeft" activeCell="A107" activeCellId="0" sqref="A107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2252,6 +2255,23 @@
         <v>1.12</v>
       </c>
     </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B106" s="2" t="n">
+        <v>134.2</v>
+      </c>
+      <c r="C106" s="2" t="n">
+        <v>133.3</v>
+      </c>
+      <c r="D106" s="2" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="E106" s="2" t="n">
+        <v>1.15</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/15 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/15</t>
   </si>
 </sst>
 </file>
@@ -456,13 +459,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A107" activeCellId="0" sqref="A107"/>
+      <selection pane="topLeft" activeCell="A108" activeCellId="0" sqref="A108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2272,6 +2275,23 @@
         <v>1.15</v>
       </c>
     </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B107" s="2" t="n">
+        <v>156.5</v>
+      </c>
+      <c r="C107" s="2" t="n">
+        <v>155.3</v>
+      </c>
+      <c r="D107" s="2" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="E107" s="2" t="n">
+        <v>1.17</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/17 and 2021/11/18 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/17</t>
   </si>
 </sst>
 </file>
@@ -459,13 +462,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A108" activeCellId="0" sqref="A108"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A109" activeCellId="0" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2292,6 +2295,23 @@
         <v>1.17</v>
       </c>
     </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B108" s="2" t="n">
+        <v>173.7</v>
+      </c>
+      <c r="C108" s="2" t="n">
+        <v>172.9</v>
+      </c>
+      <c r="D108" s="2" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E108" s="2" t="n">
+        <v>1.17</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/19 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/19</t>
   </si>
 </sst>
 </file>
@@ -462,13 +465,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A109" activeCellId="0" sqref="A109"/>
+      <selection pane="topLeft" activeCell="A110" activeCellId="0" sqref="A110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2312,6 +2315,23 @@
         <v>1.17</v>
       </c>
     </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B109" s="2" t="n">
+        <v>191.2</v>
+      </c>
+      <c r="C109" s="2" t="n">
+        <v>190.9</v>
+      </c>
+      <c r="D109" s="2" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E109" s="2" t="n">
+        <v>1.18</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/21 and 2021/11/22 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/22</t>
   </si>
 </sst>
 </file>
@@ -465,13 +468,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A110" activeCellId="0" sqref="A110"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A111" activeCellId="0" sqref="A111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.36328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2332,6 +2335,23 @@
         <v>1.18</v>
       </c>
     </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B110" s="2" t="n">
+        <v>228.9</v>
+      </c>
+      <c r="C110" s="2" t="n">
+        <v>228.8</v>
+      </c>
+      <c r="D110" s="2" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="E110" s="2" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/24 and 2021/11/25 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/24</t>
   </si>
 </sst>
 </file>
@@ -468,13 +471,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A111" activeCellId="0" sqref="A111"/>
+      <selection pane="topLeft" activeCell="A112" activeCellId="0" sqref="A112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.36328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2352,6 +2355,23 @@
         <v>1.2</v>
       </c>
     </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B111" s="2" t="n">
+        <v>251.1</v>
+      </c>
+      <c r="C111" s="2" t="n">
+        <v>251.3</v>
+      </c>
+      <c r="D111" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="E111" s="2" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/26 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/26</t>
   </si>
 </sst>
 </file>
@@ -471,13 +474,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A112" activeCellId="0" sqref="A112"/>
+      <selection pane="topLeft" activeCell="A113" activeCellId="0" sqref="A113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.3984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2372,6 +2375,23 @@
         <v>1.2</v>
       </c>
     </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B112" s="2" t="n">
+        <v>279.8</v>
+      </c>
+      <c r="C112" s="2" t="n">
+        <v>280.2</v>
+      </c>
+      <c r="D112" s="2" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="E112" s="2" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/11/29 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/11/29</t>
   </si>
 </sst>
 </file>
@@ -474,13 +477,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A113" activeCellId="0" sqref="A113"/>
+      <selection pane="topLeft" activeCell="A114" activeCellId="0" sqref="A114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.3984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2392,6 +2395,23 @@
         <v>1.2</v>
       </c>
     </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B113" s="2" t="n">
+        <v>325.9</v>
+      </c>
+      <c r="C113" s="2" t="n">
+        <v>327.5</v>
+      </c>
+      <c r="D113" s="2" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E113" s="2" t="n">
+        <v>1.18</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/01 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/11/29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/01</t>
   </si>
 </sst>
 </file>
@@ -477,13 +480,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A114" activeCellId="0" sqref="A114"/>
+      <selection pane="topLeft" activeCell="A115" activeCellId="0" sqref="A115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2412,6 +2415,23 @@
         <v>1.18</v>
       </c>
     </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B114" s="2" t="n">
+        <v>349.8</v>
+      </c>
+      <c r="C114" s="2" t="n">
+        <v>351.4</v>
+      </c>
+      <c r="D114" s="2" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="E114" s="2" t="n">
+        <v>1.16</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/03 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -374,6 +374,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/12/01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/03</t>
   </si>
 </sst>
 </file>
@@ -480,13 +483,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A115" activeCellId="0" sqref="A115"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2432,6 +2435,23 @@
         <v>1.16</v>
       </c>
     </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B115" s="2" t="n">
+        <v>374</v>
+      </c>
+      <c r="C115" s="2" t="n">
+        <v>376.5</v>
+      </c>
+      <c r="D115" s="2" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E115" s="2" t="n">
+        <v>1.14</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/06, 2021/12/07 and 2021/12/08 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -377,6 +377,12 @@
   </si>
   <si>
     <t xml:space="preserve">2021/12/03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/08</t>
   </si>
 </sst>
 </file>
@@ -483,13 +489,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
+      <selection pane="topLeft" activeCell="A118" activeCellId="0" sqref="A118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2452,6 +2458,40 @@
         <v>1.14</v>
       </c>
     </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B116" s="2" t="n">
+        <v>410.4</v>
+      </c>
+      <c r="C116" s="2" t="n">
+        <v>413.9</v>
+      </c>
+      <c r="D116" s="2" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E116" s="2" t="n">
+        <v>1.11</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B117" s="2" t="n">
+        <v>438.4</v>
+      </c>
+      <c r="C117" s="2" t="n">
+        <v>442.1</v>
+      </c>
+      <c r="D117" s="2" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="E117" s="2" t="n">
+        <v>1.11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/10 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/12/08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/10</t>
   </si>
 </sst>
 </file>
@@ -489,13 +492,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A118" activeCellId="0" sqref="A118"/>
+      <selection pane="topLeft" activeCell="A119" activeCellId="0" sqref="A119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2492,6 +2495,23 @@
         <v>1.11</v>
       </c>
     </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B118" s="2" t="n">
+        <v>457.7</v>
+      </c>
+      <c r="C118" s="2" t="n">
+        <v>462.5</v>
+      </c>
+      <c r="D118" s="2" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="E118" s="2" t="n">
+        <v>1.11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/13 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -492,13 +492,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A119" activeCellId="0" sqref="A119"/>
+      <selection pane="topLeft" activeCell="A120" activeCellId="0" sqref="A120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2512,6 +2512,23 @@
         <v>1.11</v>
       </c>
     </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B119" s="2" t="n">
+        <v>485.3</v>
+      </c>
+      <c r="C119" s="2" t="n">
+        <v>490.3</v>
+      </c>
+      <c r="D119" s="2" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E119" s="2" t="n">
+        <v>1.09</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/15 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/12/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/15</t>
   </si>
 </sst>
 </file>
@@ -492,13 +495,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A120" activeCellId="0" sqref="A120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2529,6 +2532,23 @@
         <v>1.09</v>
       </c>
     </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B120" s="2" t="n">
+        <v>508.8</v>
+      </c>
+      <c r="C120" s="2" t="n">
+        <v>514.4</v>
+      </c>
+      <c r="D120" s="2" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="E120" s="2" t="n">
+        <v>1.08</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/16 and 2021/12/17 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="124">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -389,6 +389,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/12/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/17</t>
   </si>
 </sst>
 </file>
@@ -495,13 +498,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A120" activeCellId="0" sqref="A120"/>
+      <selection pane="topLeft" activeCell="A122" activeCellId="0" sqref="A122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2549,6 +2552,23 @@
         <v>1.08</v>
       </c>
     </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B121" s="2" t="n">
+        <v>525.5</v>
+      </c>
+      <c r="C121" s="2" t="n">
+        <v>531.2</v>
+      </c>
+      <c r="D121" s="2" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="E121" s="2" t="n">
+        <v>1.07</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/19 and 2021/12/20 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="125">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -392,6 +392,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/12/17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/20</t>
   </si>
 </sst>
 </file>
@@ -498,13 +501,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A122" activeCellId="0" sqref="A122"/>
+      <selection pane="topLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2569,6 +2572,23 @@
         <v>1.07</v>
       </c>
     </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B122" s="2" t="n">
+        <v>558.5</v>
+      </c>
+      <c r="C122" s="2" t="n">
+        <v>562.3</v>
+      </c>
+      <c r="D122" s="2" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="E122" s="2" t="n">
+        <v>1.06</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/22, 2021/12/23 and 2021/12/24 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -395,6 +395,12 @@
   </si>
   <si>
     <t xml:space="preserve">2021/12/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/24</t>
   </si>
 </sst>
 </file>
@@ -501,13 +507,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A125" activeCellId="0" sqref="A125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2589,6 +2595,40 @@
         <v>1.06</v>
       </c>
     </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B123" s="2" t="n">
+        <v>579.3</v>
+      </c>
+      <c r="C123" s="2" t="n">
+        <v>582.3</v>
+      </c>
+      <c r="D123" s="2" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="E123" s="2" t="n">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B124" s="2" t="n">
+        <v>630.8</v>
+      </c>
+      <c r="C124" s="2" t="n">
+        <v>633.1</v>
+      </c>
+      <c r="D124" s="2" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="E124" s="2" t="n">
+        <v>1.11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/27 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/12/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/27</t>
   </si>
 </sst>
 </file>
@@ -507,13 +510,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A125" activeCellId="0" sqref="A125"/>
+      <selection pane="topLeft" activeCell="A126" activeCellId="0" sqref="A126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.59765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2629,6 +2632,23 @@
         <v>1.11</v>
       </c>
     </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B125" s="2" t="n">
+        <v>804.3</v>
+      </c>
+      <c r="C125" s="2" t="n">
+        <v>807.4</v>
+      </c>
+      <c r="D125" s="2" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="E125" s="2" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/29 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="129">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -404,6 +404,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/12/27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/29</t>
   </si>
 </sst>
 </file>
@@ -510,13 +513,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A126" activeCellId="0" sqref="A126"/>
+      <selection pane="topLeft" activeCell="A127" activeCellId="0" sqref="A127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.59765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2649,6 +2652,23 @@
         <v>1.23</v>
       </c>
     </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B126" s="2" t="n">
+        <v>923.4</v>
+      </c>
+      <c r="C126" s="2" t="n">
+        <v>927.6</v>
+      </c>
+      <c r="D126" s="2" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="E126" s="2" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2021/12/31 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="130">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/12/29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/12/31</t>
   </si>
 </sst>
 </file>
@@ -513,13 +516,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E126"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A127" activeCellId="0" sqref="A127"/>
+      <selection pane="topLeft" activeCell="A128" activeCellId="0" sqref="A128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2669,6 +2672,23 @@
         <v>1.3</v>
       </c>
     </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B127" s="2" t="n">
+        <v>1182.7</v>
+      </c>
+      <c r="C127" s="2" t="n">
+        <v>1188.4</v>
+      </c>
+      <c r="D127" s="2" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E127" s="2" t="n">
+        <v>1.36</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/03 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -410,6 +410,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021/12/31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/03</t>
   </si>
 </sst>
 </file>
@@ -516,13 +519,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A128" activeCellId="0" sqref="A128"/>
+      <selection pane="topLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2689,6 +2692,23 @@
         <v>1.36</v>
       </c>
     </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B128" s="2" t="n">
+        <v>1805.2</v>
+      </c>
+      <c r="C128" s="2" t="n">
+        <v>1817.3</v>
+      </c>
+      <c r="D128" s="2" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="E128" s="2" t="n">
+        <v>1.43</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/05 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="132">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/01/03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/05</t>
   </si>
 </sst>
 </file>
@@ -519,13 +522,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
+      <selection pane="topLeft" activeCell="A130" activeCellId="0" sqref="A130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2709,6 +2712,23 @@
         <v>1.43</v>
       </c>
     </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B129" s="2" t="n">
+        <v>2104.7</v>
+      </c>
+      <c r="C129" s="2" t="n">
+        <v>2114.3</v>
+      </c>
+      <c r="D129" s="2" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="E129" s="2" t="n">
+        <v>1.41</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/10, 2022/01/11 and 2020/01/12 reports. - Empty data on 2022/01/06, 2022/01/07, 2022/01/08 and 2022/01/09 due to the reports have not been published as usual.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="134">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -416,6 +416,12 @@
   </si>
   <si>
     <t xml:space="preserve">2022/01/05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/12</t>
   </si>
 </sst>
 </file>
@@ -522,13 +528,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E129"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A130" activeCellId="0" sqref="A130"/>
+      <selection pane="topLeft" activeCell="A132" activeCellId="0" sqref="A132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2729,6 +2735,40 @@
         <v>1.41</v>
       </c>
     </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B130" s="2" t="n">
+        <v>3204.4</v>
+      </c>
+      <c r="C130" s="2" t="n">
+        <v>3209.1</v>
+      </c>
+      <c r="D130" s="2" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E130" s="2" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B131" s="2" t="n">
+        <v>3615.9</v>
+      </c>
+      <c r="C131" s="2" t="n">
+        <v>3615.3</v>
+      </c>
+      <c r="D131" s="2" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="E131" s="2" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/06, 2022/01/07, 2022/01/08 and 2022/01/09 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="135">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -416,6 +416,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/01/05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/07</t>
   </si>
   <si>
     <t xml:space="preserve">2022/01/10</t>
@@ -528,13 +531,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A132" activeCellId="0" sqref="A132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2740,16 +2743,16 @@
         <v>132</v>
       </c>
       <c r="B130" s="2" t="n">
-        <v>3204.4</v>
+        <v>2438.8</v>
       </c>
       <c r="C130" s="2" t="n">
-        <v>3209.1</v>
+        <v>2444.5</v>
       </c>
       <c r="D130" s="2" t="n">
-        <v>1.24</v>
+        <v>1.32</v>
       </c>
       <c r="E130" s="2" t="n">
-        <v>1.24</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2757,15 +2760,32 @@
         <v>133</v>
       </c>
       <c r="B131" s="2" t="n">
+        <v>3204.4</v>
+      </c>
+      <c r="C131" s="2" t="n">
+        <v>3209.1</v>
+      </c>
+      <c r="D131" s="2" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E131" s="2" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B132" s="2" t="n">
         <v>3615.9</v>
       </c>
-      <c r="C131" s="2" t="n">
+      <c r="C132" s="2" t="n">
         <v>3615.3</v>
       </c>
-      <c r="D131" s="2" t="n">
+      <c r="D132" s="2" t="n">
         <v>1.23</v>
       </c>
-      <c r="E131" s="2" t="n">
+      <c r="E132" s="2" t="n">
         <v>1.23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/14 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="136">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -425,6 +425,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/01/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/14</t>
   </si>
 </sst>
 </file>
@@ -531,13 +534,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A132" activeCellId="0" sqref="A132"/>
+      <selection pane="topLeft" activeCell="A134" activeCellId="0" sqref="A134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2789,6 +2792,23 @@
         <v>1.23</v>
       </c>
     </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B133" s="2" t="n">
+        <v>3813.6</v>
+      </c>
+      <c r="C133" s="2" t="n">
+        <v>3796</v>
+      </c>
+      <c r="D133" s="2" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="E133" s="2" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/17 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -428,6 +428,12 @@
   </si>
   <si>
     <t xml:space="preserve">2022/01/14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;3840</t>
   </si>
 </sst>
 </file>
@@ -534,13 +540,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E133"/>
+  <dimension ref="A1:E134"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A134" activeCellId="0" sqref="A134"/>
+      <selection pane="topLeft" activeCell="A135" activeCellId="0" sqref="A135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2809,6 +2815,23 @@
         <v>1.19</v>
       </c>
     </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D134" s="2" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E134" s="2" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/19 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="139">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t xml:space="preserve">&gt;3840</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/19</t>
   </si>
 </sst>
 </file>
@@ -540,13 +543,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A135" activeCellId="0" sqref="A135"/>
+      <selection pane="topLeft" activeCell="A136" activeCellId="0" sqref="A136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2832,6 +2835,23 @@
         <v>1.3</v>
       </c>
     </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B135" s="2" t="n">
+        <v>4490.9</v>
+      </c>
+      <c r="C135" s="2" t="n">
+        <v>4437.4</v>
+      </c>
+      <c r="D135" s="2" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="E135" s="2" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/21 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="140">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/01/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/21</t>
   </si>
 </sst>
 </file>
@@ -543,13 +546,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E136"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A136" activeCellId="0" sqref="A136"/>
+      <selection pane="topLeft" activeCell="A137" activeCellId="0" sqref="A137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2852,6 +2855,23 @@
         <v>1.1</v>
       </c>
     </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B136" s="2" t="n">
+        <v>4731.3</v>
+      </c>
+      <c r="C136" s="2" t="n">
+        <v>4674</v>
+      </c>
+      <c r="D136" s="2" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E136" s="2" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/24 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="141">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -440,6 +440,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/01/21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/24</t>
   </si>
 </sst>
 </file>
@@ -546,13 +549,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:E137"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A137" activeCellId="0" sqref="A137"/>
+      <selection pane="topLeft" activeCell="A138" activeCellId="0" sqref="A138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2872,6 +2875,23 @@
         <v>1.1</v>
       </c>
     </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B137" s="2" t="n">
+        <v>5322.6</v>
+      </c>
+      <c r="C137" s="2" t="n">
+        <v>5262.8</v>
+      </c>
+      <c r="D137" s="2" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="E137" s="2" t="n">
+        <v>1.15</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/26 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -443,6 +443,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/01/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/26</t>
   </si>
 </sst>
 </file>
@@ -549,13 +552,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:E138"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A138" activeCellId="0" sqref="A138"/>
+      <selection pane="topLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2892,6 +2895,23 @@
         <v>1.15</v>
       </c>
     </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B138" s="2" t="n">
+        <v>5728.4</v>
+      </c>
+      <c r="C138" s="2" t="n">
+        <v>5683.5</v>
+      </c>
+      <c r="D138" s="2" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E138" s="2" t="n">
+        <v>1.18</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/28 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="143">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -446,6 +446,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/01/26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/28</t>
   </si>
 </sst>
 </file>
@@ -552,13 +555,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E138"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
+      <selection pane="topLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2912,6 +2915,23 @@
         <v>1.18</v>
       </c>
     </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B139" s="2" t="n">
+        <v>6130.9</v>
+      </c>
+      <c r="C139" s="2" t="n">
+        <v>6108.7</v>
+      </c>
+      <c r="D139" s="2" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="E139" s="2" t="n">
+        <v>1.17</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/01/31 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="144">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/01/28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/01/31</t>
   </si>
 </sst>
 </file>
@@ -555,13 +558,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
+      <selection pane="topLeft" activeCell="A141" activeCellId="0" sqref="A141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2932,6 +2935,23 @@
         <v>1.17</v>
       </c>
     </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B140" s="2" t="n">
+        <v>6836.6</v>
+      </c>
+      <c r="C140" s="2" t="n">
+        <v>6848.7</v>
+      </c>
+      <c r="D140" s="2" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E140" s="2" t="n">
+        <v>1.14</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/02 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="145">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/01/31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/02</t>
   </si>
 </sst>
 </file>
@@ -558,13 +561,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E140"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A141" activeCellId="0" sqref="A141"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A142" activeCellId="0" sqref="A142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2952,6 +2955,23 @@
         <v>1.14</v>
       </c>
     </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B141" s="2" t="n">
+        <v>7081.7</v>
+      </c>
+      <c r="C141" s="2" t="n">
+        <v>7111.8</v>
+      </c>
+      <c r="D141" s="2" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E141" s="2" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/04 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -455,6 +455,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/04</t>
   </si>
 </sst>
 </file>
@@ -561,13 +564,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A142" activeCellId="0" sqref="A142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2972,6 +2975,23 @@
         <v>1.1</v>
       </c>
     </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B142" s="2" t="n">
+        <v>7163.7</v>
+      </c>
+      <c r="C142" s="2" t="n">
+        <v>7207</v>
+      </c>
+      <c r="D142" s="2" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="E142" s="2" t="n">
+        <v>1.05</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/07 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="147">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/07</t>
   </si>
 </sst>
 </file>
@@ -564,13 +567,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E142"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A142" activeCellId="0" sqref="A142"/>
+      <selection pane="topLeft" activeCell="A143" activeCellId="0" sqref="A143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -2992,6 +2995,23 @@
         <v>1.05</v>
       </c>
     </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B143" s="2" t="n">
+        <v>6901</v>
+      </c>
+      <c r="C143" s="2" t="n">
+        <v>6953.7</v>
+      </c>
+      <c r="D143" s="2" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="E143" s="2" t="n">
+        <v>0.97</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/09 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="148">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/09</t>
   </si>
 </sst>
 </file>
@@ -567,13 +570,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:E144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A143" activeCellId="0" sqref="A143"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A145" activeCellId="0" sqref="A145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3012,6 +3015,23 @@
         <v>0.97</v>
       </c>
     </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B144" s="2" t="n">
+        <v>6562.1</v>
+      </c>
+      <c r="C144" s="2" t="n">
+        <v>6610.1</v>
+      </c>
+      <c r="D144" s="2" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="E144" s="2" t="n">
+        <v>0.92</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/11 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="149">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -464,6 +464,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/11</t>
   </si>
 </sst>
 </file>
@@ -570,13 +573,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E144"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A145" activeCellId="0" sqref="A145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3032,6 +3035,23 @@
         <v>0.92</v>
       </c>
     </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B145" s="2" t="n">
+        <v>6099.6</v>
+      </c>
+      <c r="C145" s="2" t="n">
+        <v>6133</v>
+      </c>
+      <c r="D145" s="2" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="E145" s="2" t="n">
+        <v>0.88</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/14 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="150">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -467,6 +467,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/14</t>
   </si>
 </sst>
 </file>
@@ -573,13 +576,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:E146"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A145" activeCellId="0" sqref="A145"/>
+      <selection pane="topLeft" activeCell="A147" activeCellId="0" sqref="A147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3052,6 +3055,23 @@
         <v>0.88</v>
       </c>
     </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B146" s="2" t="n">
+        <v>4989.6</v>
+      </c>
+      <c r="C146" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="D146" s="2" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="E146" s="2" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/16 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="151">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/16</t>
   </si>
 </sst>
 </file>
@@ -576,13 +579,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A147" activeCellId="0" sqref="A147"/>
+      <selection pane="topLeft" activeCell="A148" activeCellId="0" sqref="A148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3072,6 +3075,23 @@
         <v>0.8</v>
       </c>
     </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B147" s="2" t="n">
+        <v>4390.9</v>
+      </c>
+      <c r="C147" s="2" t="n">
+        <v>4385.9</v>
+      </c>
+      <c r="D147" s="2" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="E147" s="2" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/18 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="152">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/18</t>
   </si>
 </sst>
 </file>
@@ -579,13 +582,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E148"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A148" activeCellId="0" sqref="A148"/>
+      <selection pane="topLeft" activeCell="A149" activeCellId="0" sqref="A149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3092,6 +3095,23 @@
         <v>0.75</v>
       </c>
     </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B148" s="2" t="n">
+        <v>3853.1</v>
+      </c>
+      <c r="C148" s="2" t="n">
+        <v>3833.4</v>
+      </c>
+      <c r="D148" s="2" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="E148" s="2" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/21 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="153">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -476,6 +476,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/21</t>
   </si>
 </sst>
 </file>
@@ -582,13 +585,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E148"/>
+  <dimension ref="A1:E149"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A149" activeCellId="0" sqref="A149"/>
+      <selection pane="topLeft" activeCell="A150" activeCellId="0" sqref="A150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.01171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3112,6 +3115,23 @@
         <v>0.73</v>
       </c>
     </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B149" s="2" t="n">
+        <v>2934</v>
+      </c>
+      <c r="C149" s="2" t="n">
+        <v>2890.9</v>
+      </c>
+      <c r="D149" s="2" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="E149" s="2" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/23 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="154">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/23</t>
   </si>
 </sst>
 </file>
@@ -585,13 +588,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E149"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A150" activeCellId="0" sqref="A150"/>
+      <selection pane="topLeft" activeCell="A151" activeCellId="0" sqref="A151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.01171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3132,6 +3135,23 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B150" s="2" t="n">
+        <v>2533.7</v>
+      </c>
+      <c r="C150" s="2" t="n">
+        <v>2470.4</v>
+      </c>
+      <c r="D150" s="2" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="E150" s="2" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/25 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="155">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/25</t>
   </si>
 </sst>
 </file>
@@ -588,13 +591,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A151" activeCellId="0" sqref="A151"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A152" activeCellId="0" sqref="A152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3152,6 +3155,23 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B151" s="2" t="n">
+        <v>2222.5</v>
+      </c>
+      <c r="C151" s="2" t="n">
+        <v>2157.4</v>
+      </c>
+      <c r="D151" s="2" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="E151" s="2" t="n">
+        <v>0.71</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/02/28 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="156">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -485,6 +485,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/02/28</t>
   </si>
 </sst>
 </file>
@@ -591,13 +594,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A152" activeCellId="0" sqref="A152"/>
+      <selection pane="topLeft" activeCell="A153" activeCellId="0" sqref="A153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.06640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3172,6 +3175,23 @@
         <v>0.71</v>
       </c>
     </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B152" s="2" t="n">
+        <v>1806.8</v>
+      </c>
+      <c r="C152" s="2" t="n">
+        <v>1728</v>
+      </c>
+      <c r="D152" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E152" s="2" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/03/02 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -488,6 +488,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/02/28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/03/02</t>
   </si>
 </sst>
 </file>
@@ -594,13 +597,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A153" activeCellId="0" sqref="A153"/>
+      <selection pane="topLeft" activeCell="A154" activeCellId="0" sqref="A154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.06640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3192,6 +3195,23 @@
         <v>0.73</v>
       </c>
     </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B153" s="2" t="n">
+        <v>1638.1</v>
+      </c>
+      <c r="C153" s="2" t="n">
+        <v>1557.3</v>
+      </c>
+      <c r="D153" s="2" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="E153" s="2" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/03/04 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="158">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -491,6 +491,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/03/02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/03/04</t>
   </si>
 </sst>
 </file>
@@ -597,13 +600,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E153"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A154" activeCellId="0" sqref="A154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.1015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3212,6 +3215,23 @@
         <v>0.75</v>
       </c>
     </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B154" s="2" t="n">
+        <v>1512.7</v>
+      </c>
+      <c r="C154" s="2" t="n">
+        <v>1432.4</v>
+      </c>
+      <c r="D154" s="2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="E154" s="2" t="n">
+        <v>0.76</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/03/07 and 2022/03/08 reports.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="159">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/03/04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/03/07</t>
   </si>
 </sst>
 </file>
@@ -600,13 +603,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E155"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A154" activeCellId="0" sqref="A154"/>
+      <selection pane="topLeft" activeCell="A156" activeCellId="0" sqref="A156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.1015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3232,6 +3235,23 @@
         <v>0.76</v>
       </c>
     </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B155" s="2" t="n">
+        <v>1398.1</v>
+      </c>
+      <c r="C155" s="2" t="n">
+        <v>1316.3</v>
+      </c>
+      <c r="D155" s="2" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="E155" s="2" t="n">
+        <v>0.83</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
- Data update from DGS's 2022/03/09 report.
</commit_message>
<xml_diff>
--- a/risk_matrix_time_series.xlsx
+++ b/risk_matrix_time_series.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="160">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -497,6 +497,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022/03/07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/03/09</t>
   </si>
 </sst>
 </file>
@@ -603,13 +606,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E155"/>
+  <dimension ref="A1:E156"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A156" activeCellId="0" sqref="A156"/>
+      <selection pane="topLeft" activeCell="A157" activeCellId="0" sqref="A157"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.06"/>
@@ -3252,6 +3255,23 @@
         <v>0.83</v>
       </c>
     </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B156" s="2" t="n">
+        <v>1411.2</v>
+      </c>
+      <c r="C156" s="2" t="n">
+        <v>1330.6</v>
+      </c>
+      <c r="D156" s="2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="E156" s="2" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>